<commit_message>
Updated Game Plan Excel File
No changes made to .pages file, excel file updated to what I had written by last class in the pages file though.
</commit_message>
<xml_diff>
--- a/Game Plan.xlsx
+++ b/Game Plan.xlsx
@@ -12,9 +12,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="26">
-  <si>
-    <t>Character is a scientist who discovered that the world is actually flat. He knew this would anger a great many people so he decided to keep this finding to himself, aside from telling his own mother, of course. When he woke up however, he discovers that the information got out.</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="27">
+  <si>
+    <t>Character is a scientist who discovered that the world is actually flat. He knew this would anger a great many people so he decided to keep this finding to himself, aside from telling his own mother, of course. When he woke up however, he discovers that the information got out. You must find and destroy the paper before the angry mobs do or an even worse chaos will ensue.</t>
   </si>
   <si>
     <t>Levels</t>
@@ -26,7 +26,7 @@
     <t>Mission</t>
   </si>
   <si>
-    <t xml:space="preserve">Cut Scenes / Hint Bubbles </t>
+    <t>Cut Scenes / Hint Bubbles / Dialog</t>
   </si>
   <si>
     <r>
@@ -105,7 +105,26 @@
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
       </rPr>
-      <t xml:space="preserve">— Character gets a call from his/her mother saying she published his scientific findings against his wishes — character says </t>
+      <t xml:space="preserve">— “Last night we received a tip from a source who wishes to remain anonymous stating that **Characters name** has scientific proof that the world is actually flat.” - </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>news dialog</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve"> + +— Character gets a call from his/her mother saying she published his scientific findings against his wishes — character says </t>
     </r>
     <r>
       <rPr>
@@ -134,7 +153,7 @@
         <rFont val="Helvetica Neue"/>
       </rPr>
       <t> -— (After first visit to lab) When returning to house he/she gets a call from his/her mother saying the publisher won’t withdrawal the article and that the character will have to go there and force their hand</t>
+— “I gave the publisher a call. They said they won’t withdrawal the article. The address for the publishers office is… Oh the angry mob on your roof cut your power lines and your phone got soaked going through the sewer so now you can’t use GoogleMaps? I’ll print you off a map then. Head here after you get the research paper from the lab so that you can pick it up.”</t>
     </r>
   </si>
   <si>
@@ -248,16 +267,18 @@
     <t>Moms Place</t>
   </si>
   <si>
-    <t>— Old lady’s house.. cats everywhere.. idk</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t xml:space="preserve">— Character will need to convince his mother to relinquish rights for the publication of his findings from the publisher
+    <t>— Old lady’s house. Cats everywhere.. + +</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve">— Mom does not remember where the she left the publishers number, but she has a story to tell you about her night that might give you a hint
 </t>
     </r>
     <r>
@@ -275,19 +296,12 @@
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
       </rPr>
-      <t xml:space="preserve">— Must talk sense into mother (picking from a list of pre-made responses) to convince her to call publisher while avoiding making her angry and getting smacked </t>
+      <t>— Must listen to old lady mom’s story and deduce which cats snatched the piece of paper with the publishers number on it to advance  +</t>
     </r>
     <r>
       <rPr>
         <b val="1"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t>(Health bar level)</t>
-    </r>
-    <r>
-      <rPr>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -297,6 +311,14 @@
     </r>
     <r>
       <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>— Character will need to make it to the lab in order to destroy evidence of his scientific findings</t>
+    </r>
+    <r>
+      <rPr>
         <b val="1"/>
         <sz val="10"/>
         <color indexed="8"/>
@@ -305,13 +327,15 @@
       <t>  </t>
     </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t>— Character will need to make it to the lab in order to destroy evidence of his scientific findings</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve">— Mob has moved on to the lab in order to find and disprove the paper. However, the ones who somehow found their way to the roof didn’t plan a way to get down. They are stuck there. - </t>
     </r>
     <r>
       <rPr>
@@ -320,50 +344,10 @@
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
       </rPr>
-      <t> -</t>
-    </r>
-  </si>
-  <si>
-    <t>— “Take this wooden cane in case you run into any trouble” — mom</t>
-  </si>
-  <si>
-    <t>Lab</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t>— Angry mob outside blocking the way is too large to fight off. - -</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t>— Lands on the roof with helicopter and there are several people inside the lab looting it, trying to find the research</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t>— Must return to house and fight off the mob with moms cane get to the helicopter to enter the lab through the roof - -— Character needs to find and destroy the evidence and then head back to “moms place” to get a map to find the publisher</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="1"/>
+      <t>dialog</t>
+    </r>
+    <r>
+      <rPr>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -371,6 +355,123 @@
       <t xml:space="preserve">  
 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve">— “The lady on the news says the angry mob moved to your lab. Good thing you always lock up. You’re going to have to make it to your lab and pick up that paper before they get it if you really think it would be dangerous for someone to have proof. Take this wooden cane in case you run into any trouble” — </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>mom</t>
+    </r>
+  </si>
+  <si>
+    <t>Lab</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>— The way to the lab is blocked by an angry mob + +</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>— Lands on the roof with helicopter and there are several people inside the lab looting it, trying to find the research in order to disprove it</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>— Must return to house and fight off the roof mob with moms cane and get to the helicopter to enter the lab through the roof + +</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>— Character needs to find where people are getting in and block the way before he can open his safe and destroy the evidence. Then the character must head back to “moms place” to get a map to find the publisher.</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve"> +
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve">— Angry mob outside blocking the way is too large to fight off - </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>dialog + +</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve">— There are people inside. You must have left one of the windows open or something. Let’s find where they’re getting in and block it before we get overwhelmed. - </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>dialog</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
     </r>
   </si>
   <si>
@@ -1690,7 +1791,7 @@
     <col min="5" max="256" width="16.3516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="71.1" customHeight="1">
+    <row r="1" ht="78" customHeight="1">
       <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
@@ -1712,7 +1813,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" ht="158.7" customHeight="1">
+    <row r="3" ht="282.2" customHeight="1">
       <c r="A3" t="s" s="4">
         <v>5</v>
       </c>
@@ -1762,7 +1863,7 @@
       </c>
       <c r="D6" s="10"/>
     </row>
-    <row r="7" ht="188.15" customHeight="1">
+    <row r="7" ht="176.1" customHeight="1">
       <c r="A7" t="s" s="7">
         <v>18</v>
       </c>
@@ -1776,7 +1877,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" ht="140.1" customHeight="1">
+    <row r="8" ht="164.1" customHeight="1">
       <c r="A8" t="s" s="7">
         <v>22</v>
       </c>
@@ -1786,11 +1887,13 @@
       <c r="C8" t="s" s="9">
         <v>24</v>
       </c>
-      <c r="D8" s="10"/>
+      <c r="D8" t="s" s="9">
+        <v>25</v>
+      </c>
     </row>
     <row r="9" ht="20.05" customHeight="1">
       <c r="A9" t="s" s="7">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B9" s="11"/>
       <c r="C9" s="10"/>

</xml_diff>